<commit_message>
-New SSH logic -Added local reporting system -System of parallel control of servers -New conditions for selection of whitelists -Fixed minor bugs -New UI design -Added a separate thread for processing Graffiti
</commit_message>
<xml_diff>
--- a/GraffitiChanger/GraffitiChanger/bin/Debug/net5.0-windows/data.xlsx
+++ b/GraffitiChanger/GraffitiChanger/bin/Debug/net5.0-windows/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasha\source\repos\GraffitiChanger\GraffitiChanger\bin\Debug\net5.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasha\source\repos\GraffitiAutomatization\GraffitiChanger\GraffitiChanger\bin\Debug\net5.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DADD83C3-17EE-4F6C-9112-065F57505022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0308584F-A123-4686-A4F6-CA7B98CCF3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{994BC8D2-F2AF-427B-A502-C115428CAC9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>IP</t>
   </si>
@@ -44,7 +44,10 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>MOHITO</t>
+    <t>tvhome</t>
+  </si>
+  <si>
+    <t>KOLA</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877A0F91-01C4-426D-8C86-2639F47DA2F2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +427,128 @@
         <v>123</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2345</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>124</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>623</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>45732</v>
+      </c>
+      <c r="B6">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5243</v>
+      </c>
+      <c r="B7">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>236</v>
+      </c>
+      <c r="B8">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2365</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5687</v>
+      </c>
+      <c r="B10">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>456</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6768</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>